<commit_message>
3. EntryBuilder.BuildOutputCSV对于enum类型自动设置成数值 4. 粒子系统相关修复 5. 修复Panel.ContentSizeChanged引起的死循环
</commit_message>
<xml_diff>
--- a/EntryEditor/bin/Debug/Plug-ins/EditorParticle/TEXT.xlsx
+++ b/EntryEditor/bin/Debug/Plug-ins/EditorParticle/TEXT.xlsx
@@ -24,10 +24,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>enum</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>键</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -57,10 +53,6 @@
   </si>
   <si>
     <t>重做 Ctrl+Y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>New</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -192,6 +184,14 @@
 2. 鼠标右键可拖动粒子发射器
 3. 鼠标滑轮可缩放粒子视图
 4. 键盘H键可恢复视图视角</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enum:byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New = 0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -547,7 +547,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -562,170 +562,170 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="202.5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>